<commit_message>
additional refactoring and making sure it runs
</commit_message>
<xml_diff>
--- a/model.xlsx
+++ b/model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JRobinson\udacity-dend-jr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FECC65-2E95-4ED0-A076-53EBE70B08ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999959A1-52DB-4548-9ADF-68FE9A4AAD59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28770" yWindow="30" windowWidth="28770" windowHeight="15570" xr2:uid="{86FE9C2E-42E3-4374-A81C-44BDF8C36516}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{86FE9C2E-42E3-4374-A81C-44BDF8C36516}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="67">
   <si>
     <t>fact_electricity</t>
   </si>
@@ -53,9 +53,6 @@
     <t>location_key</t>
   </si>
   <si>
-    <t>census_region_key</t>
-  </si>
-  <si>
     <t>race</t>
   </si>
   <si>
@@ -83,9 +80,6 @@
     <t>state_code</t>
   </si>
   <si>
-    <t>aer_fuel_type_key</t>
-  </si>
-  <si>
     <t>female_population</t>
   </si>
   <si>
@@ -113,18 +107,12 @@
     <t>eia_sector_desc</t>
   </si>
   <si>
-    <t>nerc_region_key</t>
-  </si>
-  <si>
     <t>average_household_size</t>
   </si>
   <si>
     <t>operator_id</t>
   </si>
   <si>
-    <t>reported_fuel_type_key</t>
-  </si>
-  <si>
     <t>count</t>
   </si>
   <si>
@@ -158,9 +146,6 @@
     <t>plant_id</t>
   </si>
   <si>
-    <t>sector_name</t>
-  </si>
-  <si>
     <t>average_temperature</t>
   </si>
   <si>
@@ -218,55 +203,40 @@
     <t>reported_prime_mover_code</t>
   </si>
   <si>
-    <t>elec_fuel_consumption</t>
-  </si>
-  <si>
     <t>day</t>
   </si>
   <si>
     <t>reported_prime_mover_desc</t>
   </si>
   <si>
-    <t>net_generation_megawatthours</t>
-  </si>
-  <si>
     <t>weekday</t>
   </si>
   <si>
     <t>balancing_authority_code</t>
   </si>
   <si>
-    <t>total_fuel_consumption_quantity</t>
-  </si>
-  <si>
     <t>balancing_authority_desc</t>
   </si>
   <si>
-    <t>electric_fuel_consumption_quantity</t>
-  </si>
-  <si>
-    <t>total_fuel_consumption_mmbtu</t>
-  </si>
-  <si>
-    <t>dim_aer_fuel_type</t>
-  </si>
-  <si>
     <t>dim_balancing_authority</t>
   </si>
   <si>
-    <t>dim_census_region</t>
-  </si>
-  <si>
     <t>dim_eia_sector</t>
   </si>
   <si>
-    <t>dim_nerc_region</t>
-  </si>
-  <si>
-    <t>dim_reported_fuel_type</t>
-  </si>
-  <si>
     <t>dim_reported_prime_mover</t>
+  </si>
+  <si>
+    <t>fuel_type_key</t>
+  </si>
+  <si>
+    <t>region_key</t>
+  </si>
+  <si>
+    <t>dim_fuel_type</t>
+  </si>
+  <si>
+    <t>dim_region</t>
   </si>
 </sst>
 </file>
@@ -629,19 +599,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7B7B48D-E233-4AF5-B574-A0DF75225729}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -649,13 +619,13 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -663,308 +633,268 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="G3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>19</v>
       </c>
-      <c r="G7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
+      <c r="E8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
       <c r="E9" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="G9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
-      </c>
-      <c r="G12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="E13" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
       </c>
-      <c r="G14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="E22" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
         <v>15</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" t="s">
-        <v>51</v>
-      </c>
-      <c r="G17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18" t="s">
-        <v>54</v>
-      </c>
-      <c r="G18" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G19" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" t="s">
-        <v>56</v>
-      </c>
-      <c r="E22" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" t="s">
-        <v>58</v>
-      </c>
-      <c r="E23" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" t="s">
-        <v>64</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>68</v>
-      </c>
-      <c r="E26" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>69</v>
-      </c>
-      <c r="E27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E28" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>